<commit_message>
2019 the open entries
</commit_message>
<xml_diff>
--- a/scripts/the-open-2019.xlsx
+++ b/scripts/the-open-2019.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="214">
   <si>
     <t xml:space="preserve">2019 PGA Championship Player Pool</t>
   </si>
@@ -634,7 +634,58 @@
     <t xml:space="preserve">Tiebreaker #2 - Total final cumulative strokes of the 2018 Champion Brooks Koepka</t>
   </si>
   <si>
-    <t xml:space="preserve">Justin Rose </t>
+    <t xml:space="preserve">Alex Duff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brett Kub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameron Weimer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curtis Chapin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dan Godshall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave Fleming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drew Serruto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ian Horwich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Donoher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin O'Brien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyle Bivenour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Marshall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick Cocalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rob Stoecklein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryan Boudouris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tim Cableck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony Boyle</t>
   </si>
 </sst>
 </file>
@@ -646,7 +697,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0%"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -751,13 +802,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -890,7 +934,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1059,10 +1103,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,26 +1183,26 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="1" sqref="C5 L16"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="2.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="2.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="2.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="2.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="16" style="0" width="9.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="2.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="2.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="9.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="23" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.5"/>
@@ -30385,7 +30425,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="9.51"/>
@@ -58635,129 +58675,922 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="5" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+      <c r="B7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="C19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="D22" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D24" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+      <c r="D29" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="41"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="41"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="41"/>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E36" s="41"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="41"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="18" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41"/>
-      <c r="F20" s="42"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="F21" s="42"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="F22" s="42"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="41"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="41"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="41"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="41"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="41"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="41"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="41"/>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="41"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="41"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A79" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D92" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D93" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>